<commit_message>
Generar Memoria Alumnos Tutor
</commit_message>
<xml_diff>
--- a/public/MD750601 Memoria Final_2DAW.xlsx
+++ b/public/MD750601 Memoria Final_2DAW.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>TUTOR:</t>
   </si>
@@ -71,6 +71,51 @@
   </si>
   <si>
     <t>APTO</t>
+  </si>
+  <si>
+    <t>Roldán Vara, Sergio</t>
+  </si>
+  <si>
+    <t>sergio@s.com</t>
+  </si>
+  <si>
+    <t>Indra Sistemas</t>
+  </si>
+  <si>
+    <t>SI/NO</t>
+  </si>
+  <si>
+    <t>Pedro Javier</t>
+  </si>
+  <si>
+    <t>Avenida de Bruselas nº 35</t>
+  </si>
+  <si>
+    <t>Alcobendas</t>
+  </si>
+  <si>
+    <t>2020-02-05</t>
+  </si>
+  <si>
+    <t>2020-12-31</t>
+  </si>
+  <si>
+    <t>NO/SI/NO EMITE</t>
+  </si>
+  <si>
+    <t>Rubio Baños, Joaquín José</t>
+  </si>
+  <si>
+    <t>rafaelangelsobrino@gmail.com</t>
+  </si>
+  <si>
+    <t>Deimos Space</t>
+  </si>
+  <si>
+    <t>Ronda de Poniente 19, – 28760</t>
+  </si>
+  <si>
+    <t>Tres Cantos</t>
   </si>
   <si>
     <t>OBSERVACIONES:</t>
@@ -1567,38 +1612,90 @@
       <c r="P5"/>
     </row>
     <row r="6" spans="1:1025">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>234234</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
       <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
+      <c r="M6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
       <c r="O6"/>
       <c r="P6"/>
     </row>
     <row r="7" spans="1:1025">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>628443211</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
       <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
+      <c r="M7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
       <c r="O7"/>
       <c r="P7"/>
     </row>
@@ -1837,7 +1934,7 @@
     </row>
     <row r="30" spans="1:1025">
       <c r="B30" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>